<commit_message>
Termine por completo el archivo relacionado con recitations week2
Ya quedo listo el recitations week2
</commit_message>
<xml_diff>
--- a/Foundations_of_modern_finance_part1/personal_exercises/week2/recitations/recitations_week2.xlsx
+++ b/Foundations_of_modern_finance_part1/personal_exercises/week2/recitations/recitations_week2.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\micro_masters_finance_mit\Foundations_of_modern_finance_part1\personal_exercises\week2\recitations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{560972BB-E2E9-4FE9-B6A7-873EF04A5A60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163F1873-8070-4263-BB6D-AA84681D9D37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{4664801A-7DB7-4C85-BD92-AD3BD8B0E02C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{4664801A-7DB7-4C85-BD92-AD3BD8B0E02C}"/>
   </bookViews>
   <sheets>
     <sheet name="question1" sheetId="1" r:id="rId1"/>
     <sheet name="question2" sheetId="2" r:id="rId2"/>
     <sheet name="question3" sheetId="3" r:id="rId3"/>
+    <sheet name="question4" sheetId="8" r:id="rId4"/>
+    <sheet name="question5" sheetId="9" r:id="rId5"/>
+    <sheet name="question6" sheetId="10" r:id="rId6"/>
+    <sheet name="question7" sheetId="12" r:id="rId7"/>
+    <sheet name="qiues" sheetId="11" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +40,93 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Lenovo</author>
+  </authors>
+  <commentList>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{AB064135-17DA-42A9-B044-3DE8DC043321}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lenovo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Prices of the different assets
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{A1D2EB50-D498-4F56-8F27-8739100E8158}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lenovo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Inverse matrix of the matrix of payoffs
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{12E3E00A-16BE-49B7-99EB-710271E6B85A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>germankux:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+state prices!!
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
   <si>
     <t>Bond</t>
   </si>
@@ -109,19 +199,162 @@
   </si>
   <si>
     <t>stock</t>
+  </si>
+  <si>
+    <t>state 1</t>
+  </si>
+  <si>
+    <t>state  2</t>
+  </si>
+  <si>
+    <t>state 3</t>
+  </si>
+  <si>
+    <t>asset 1</t>
+  </si>
+  <si>
+    <t>asset 2</t>
+  </si>
+  <si>
+    <t>asset 3</t>
+  </si>
+  <si>
+    <t>prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inverse </t>
+  </si>
+  <si>
+    <t>state  prices</t>
+  </si>
+  <si>
+    <t>Probabilities</t>
+  </si>
+  <si>
+    <t>Asset X</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Payoffs</t>
+  </si>
+  <si>
+    <t>Asset Y</t>
+  </si>
+  <si>
+    <t>FV</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV </t>
+  </si>
+  <si>
+    <t>RATE</t>
+  </si>
+  <si>
+    <t>inflation</t>
+  </si>
+  <si>
+    <t>rental revenue</t>
+  </si>
+  <si>
+    <t>real growth</t>
+  </si>
+  <si>
+    <t>real discount rate</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>nominal discount rate</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Expected rental revenue</t>
+  </si>
+  <si>
+    <t>Present Value</t>
+  </si>
+  <si>
+    <t>PV investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal growth </t>
+  </si>
+  <si>
+    <t>Method 1</t>
+  </si>
+  <si>
+    <t>Method 2</t>
+  </si>
+  <si>
+    <t>(In real terms)</t>
+  </si>
+  <si>
+    <t>(In nominal terms)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,8 +377,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +701,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +833,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,16 +911,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D31EF1-FD3B-42F2-AFA2-62FA5E6DE8AC}">
-  <dimension ref="B2:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D31EF1-FD3B-42F2-AFA2-62FA5E6DE8AC}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
       <c r="B2">
         <v>100</v>
       </c>
@@ -696,7 +951,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
       <c r="B3">
         <v>250</v>
       </c>
@@ -710,7 +968,10 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
       <c r="B4">
         <v>0</v>
       </c>
@@ -724,7 +985,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
       <c r="B6" cm="1">
         <f t="array" ref="B6:D8">MINVERSE(B2:D4)</f>
         <v>0</v>
@@ -740,7 +1004,7 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.01</v>
       </c>
@@ -754,7 +1018,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0</v>
       </c>
@@ -766,6 +1030,561 @@
       </c>
       <c r="F8">
         <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A02788F-E113-4F2F-B8E2-B3784FE81C6E}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.2</v>
+      </c>
+      <c r="C2">
+        <f xml:space="preserve"> 1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C4" si="0" xml:space="preserve"> 1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3">
+        <v>80</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <f>SUMPRODUCT(C2:C4,F2:F4)</f>
+        <v>93.333333333333314</v>
+      </c>
+      <c r="G5">
+        <f>SUMPRODUCT(C2:C4,G2:G4)</f>
+        <v>93.333333333333314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6">
+        <f>SUMPRODUCT(A2:A4,F2:F4)</f>
+        <v>84</v>
+      </c>
+      <c r="G6">
+        <f>SUMPRODUCT(A2:A4,G2:G4)</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7">
+        <f>(F5/F6 - 1) * 100</f>
+        <v>11.111111111111093</v>
+      </c>
+      <c r="G7">
+        <f>(G5/G6 - 1) * 100</f>
+        <v>2.5641025641025328</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D6D0A2-7A8A-4D43-AFFD-898EBE1628F9}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1">
+        <v>11500</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1">
+        <v>10000</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>0.08</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2">
+        <f>FV(B2,1,0,E1)</f>
+        <v>-10800</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2">
+        <f>PV(B2,1,0,B1)</f>
+        <v>-10648.148148148148</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="2">
+        <f>PV(H2,10,0,H1)</f>
+        <v>-8337.4827855243166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD886DFF-47AC-4073-BDC8-A112E2565E71}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3">
+        <f>RATE(20,0,-B1,B2)</f>
+        <v>5.6467308564940109E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2">
+        <f>FV(0.102,20,0,1)</f>
+        <v>-6.976408303330734</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2433ADEC-F1FE-4A51-B776-0F2A426FDCFF}">
+  <dimension ref="A1:P11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1">
+        <v>650000</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="2">
+        <f>FV(B2,1,0,B1)</f>
+        <v>-669500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>0.03</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2">
+        <f>PV(B4,1,0,E1)</f>
+        <v>631603.77358490566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="2">
+        <f>E1 * (1+B3)</f>
+        <v>-686237.49999999988</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>0.06</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2">
+        <f>PV(B5,1,0,E3)</f>
+        <v>631603.77358490555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <f>(1+B4)*(1+B3) - 1</f>
+        <v>8.6500000000000021E-2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <f>(1+B2)*(1+B3)-1</f>
+        <v>5.5749999999999966E-2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <f>FV($B$2,D7,0,$B$1)</f>
+        <v>-669500</v>
+      </c>
+      <c r="I7" s="2">
+        <f>PV($B$4,D7,0,E7)</f>
+        <v>631603.77358490566</v>
+      </c>
+      <c r="L7" s="2">
+        <f>FV($B$6,D7,0,$B$1)</f>
+        <v>-686237.5</v>
+      </c>
+      <c r="M7" s="2">
+        <f>E7*(1+$B$3)^D7</f>
+        <v>-686237.49999999988</v>
+      </c>
+      <c r="P7" s="2">
+        <f>PV($B$5,D7,0,L7)</f>
+        <v>631603.77358490566</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <f>FV($B$2,D8,0,$B$1)</f>
+        <v>-689585</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" ref="I8:I10" si="0">PV($B$4,D8,0,E8)</f>
+        <v>613728.19508721959</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" ref="L8:L10" si="1">FV($B$6,D8,0,$B$1)</f>
+        <v>-724495.24062499998</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" ref="M8:M10" si="2">E8*(1+$B$3)^D8</f>
+        <v>-724495.24062499998</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" ref="P8:P10" si="3">PV($B$5,D8,0,L8)</f>
+        <v>613728.19508721959</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <f>FV($B$2,D9,0,$B$1)</f>
+        <v>-710272.55</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>596358.5291885247</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="1"/>
+        <v>-764885.85028984363</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="2"/>
+        <v>-764885.85028984374</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="3"/>
+        <v>596358.52918852458</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <f>FV($B$2,D10,0,$B$1)</f>
+        <v>-731580.72649999999</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>579480.45760771725</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="1"/>
+        <v>-807528.23644350236</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>-807528.23644350236</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="3"/>
+        <v>579480.45760771725</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="2">
+        <f>SUM(I7:I10)</f>
+        <v>2421170.9554683669</v>
+      </c>
+      <c r="O11" t="s">
+        <v>53</v>
+      </c>
+      <c r="P11" s="2">
+        <f>SUM(P7:P10)</f>
+        <v>2421170.9554683669</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3D0894-6E64-4402-A901-E257B4B5F257}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1">
+        <v>650000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5">
+        <v>0.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>